<commit_message>
Versão final v0.1 via MacOsx em: 2023-07-12.
</commit_message>
<xml_diff>
--- a/dados/COVID-19-E-IES-2023.xlsx
+++ b/dados/COVID-19-E-IES-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Extension/GitHub/artigo-covid-ensino-superior/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29B5A93-6132-9846-B9F8-10A4164E6F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D62DB7-80DE-EA45-8460-95E6170DCFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10960" yWindow="500" windowWidth="17840" windowHeight="16300" xr2:uid="{072D2E1B-9696-0A4D-BDC3-56180D8625E0}"/>
+    <workbookView xWindow="4160" yWindow="500" windowWidth="23040" windowHeight="16300" xr2:uid="{072D2E1B-9696-0A4D-BDC3-56180D8625E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3741" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3748" uniqueCount="547">
   <si>
     <t>Masculino</t>
   </si>
@@ -2093,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F3A87F-111F-3A4C-87CF-4E66DFD00E3B}">
   <dimension ref="A1:AZ90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD59" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="AF63" sqref="AF63"/>
+    <sheetView tabSelected="1" topLeftCell="AB4" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2381,6 +2381,9 @@
       <c r="AD2" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="AE2" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AF2" s="5" t="s">
         <v>17</v>
       </c>
@@ -2515,6 +2518,9 @@
       <c r="AD3" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="AE3" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AF3" s="5" t="s">
         <v>79</v>
       </c>
@@ -2658,6 +2664,9 @@
       <c r="AD4" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="AE4" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AF4" s="5" t="s">
         <v>79</v>
       </c>
@@ -2795,6 +2804,9 @@
       <c r="AD5" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="AE5" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AF5" s="5" t="s">
         <v>19</v>
       </c>
@@ -2932,6 +2944,9 @@
       <c r="AD6" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="AE6" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AF6" s="5" t="s">
         <v>19</v>
       </c>
@@ -3072,6 +3087,9 @@
       <c r="AD7" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="AE7" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AF7" s="5" t="s">
         <v>17</v>
       </c>
@@ -3626,8 +3644,8 @@
       <c r="AD11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AE11" s="5" t="s">
-        <v>48</v>
+      <c r="AE11" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF11" s="5" t="s">
         <v>17</v>
@@ -3900,8 +3918,8 @@
       <c r="AD13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE13" s="5" t="s">
-        <v>48</v>
+      <c r="AE13" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF13" s="5" t="s">
         <v>19</v>
@@ -4332,8 +4350,8 @@
       <c r="AD16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AE16" s="5" t="s">
-        <v>48</v>
+      <c r="AE16" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF16" s="5" t="s">
         <v>79</v>
@@ -4761,8 +4779,8 @@
       <c r="AD19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AE19" s="5" t="s">
-        <v>48</v>
+      <c r="AE19" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF19" s="5" t="s">
         <v>19</v>
@@ -5568,8 +5586,8 @@
       <c r="AD25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AE25" s="5" t="s">
-        <v>48</v>
+      <c r="AE25" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF25" s="5" t="s">
         <v>17</v>
@@ -5699,8 +5717,8 @@
       <c r="AD26" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AE26" s="5" t="s">
-        <v>48</v>
+      <c r="AE26" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF26" s="5" t="s">
         <v>17</v>
@@ -5952,8 +5970,8 @@
       <c r="AD28" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE28" s="5" t="s">
-        <v>48</v>
+      <c r="AE28" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF28" s="5" t="s">
         <v>17</v>
@@ -6089,8 +6107,8 @@
       <c r="AD29" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AE29" s="5" t="s">
-        <v>48</v>
+      <c r="AE29" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF29" s="5" t="s">
         <v>17</v>
@@ -6232,8 +6250,8 @@
       <c r="AD30" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AE30" s="5" t="s">
-        <v>48</v>
+      <c r="AE30" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF30" s="5" t="s">
         <v>19</v>
@@ -6375,8 +6393,8 @@
       <c r="AD31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE31" s="5" t="s">
-        <v>48</v>
+      <c r="AE31" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF31" s="5" t="s">
         <v>17</v>
@@ -6649,8 +6667,8 @@
       <c r="AD33" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE33" s="5" t="s">
-        <v>48</v>
+      <c r="AE33" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF33" s="5" t="s">
         <v>17</v>
@@ -6780,8 +6798,8 @@
       <c r="AD34" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AE34" s="5" t="s">
-        <v>48</v>
+      <c r="AE34" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF34" s="5" t="s">
         <v>19</v>
@@ -7075,8 +7093,8 @@
       <c r="AD36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE36" s="5" t="s">
-        <v>48</v>
+      <c r="AE36" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF36" s="5" t="s">
         <v>79</v>
@@ -7224,8 +7242,8 @@
       <c r="AD37" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE37" s="5" t="s">
-        <v>48</v>
+      <c r="AE37" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF37" s="5" t="s">
         <v>17</v>
@@ -7531,6 +7549,9 @@
       <c r="AD39" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="AE39" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AF39" s="5" t="s">
         <v>17</v>
       </c>
@@ -7677,8 +7698,8 @@
       <c r="AD40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE40" s="5" t="s">
-        <v>48</v>
+      <c r="AE40" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF40" s="5" t="s">
         <v>19</v>
@@ -7823,8 +7844,8 @@
       <c r="AD41" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE41" s="5" t="s">
-        <v>48</v>
+      <c r="AE41" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF41" s="5" t="s">
         <v>17</v>
@@ -7969,8 +7990,8 @@
       <c r="AD42" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE42" s="5" t="s">
-        <v>48</v>
+      <c r="AE42" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF42" s="5" t="s">
         <v>17</v>
@@ -8237,8 +8258,8 @@
       <c r="AD44" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE44" s="5" t="s">
-        <v>48</v>
+      <c r="AE44" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF44" s="5" t="s">
         <v>17</v>
@@ -8383,8 +8404,8 @@
       <c r="AD45" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE45" s="5" t="s">
-        <v>48</v>
+      <c r="AE45" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF45" s="5" t="s">
         <v>17</v>
@@ -8693,8 +8714,8 @@
       <c r="AD47" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE47" s="5" t="s">
-        <v>48</v>
+      <c r="AE47" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF47" s="5" t="s">
         <v>17</v>
@@ -8839,8 +8860,8 @@
       <c r="AD48" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE48" s="5" t="s">
-        <v>48</v>
+      <c r="AE48" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF48" s="5" t="s">
         <v>79</v>
@@ -9271,8 +9292,8 @@
       <c r="AD51" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AE51" s="5" t="s">
-        <v>48</v>
+      <c r="AE51" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF51" s="5" t="s">
         <v>79</v>
@@ -9405,8 +9426,8 @@
       <c r="AD52" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AE52" s="5" t="s">
-        <v>48</v>
+      <c r="AE52" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF52" s="5" t="s">
         <v>19</v>
@@ -9813,8 +9834,8 @@
       <c r="AD55" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE55" s="5" t="s">
-        <v>48</v>
+      <c r="AE55" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF55" s="5" t="s">
         <v>19</v>
@@ -9965,8 +9986,8 @@
       <c r="AD56" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE56" s="5" t="s">
-        <v>48</v>
+      <c r="AE56" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF56" s="5" t="s">
         <v>17</v>
@@ -10117,8 +10138,8 @@
       <c r="AD57" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE57" s="5" t="s">
-        <v>48</v>
+      <c r="AE57" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF57" s="5" t="s">
         <v>17</v>
@@ -10257,8 +10278,8 @@
       <c r="AD58" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE58" s="5" t="s">
-        <v>48</v>
+      <c r="AE58" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF58" s="5" t="s">
         <v>19</v>
@@ -10391,8 +10412,8 @@
       <c r="AD59" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE59" s="5" t="s">
-        <v>48</v>
+      <c r="AE59" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF59" s="5" t="s">
         <v>19</v>
@@ -10519,8 +10540,8 @@
       <c r="AD60" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE60" s="5" t="s">
-        <v>48</v>
+      <c r="AE60" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF60" s="5" t="s">
         <v>19</v>
@@ -10653,8 +10674,8 @@
       <c r="AD61" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AE61" s="5" t="s">
-        <v>48</v>
+      <c r="AE61" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF61" s="5" t="s">
         <v>17</v>
@@ -12484,7 +12505,7 @@
         <v>17</v>
       </c>
       <c r="AE74" s="2" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="AF74" s="2" t="s">
         <v>19</v>
@@ -12904,7 +12925,7 @@
         <v>79</v>
       </c>
       <c r="AE77" s="2" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="AF77" s="2" t="s">
         <v>19</v>
@@ -13444,7 +13465,7 @@
         <v>17</v>
       </c>
       <c r="AE81" s="2" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="AF81" s="2" t="s">
         <v>19</v>
@@ -13740,7 +13761,7 @@
         <v>21</v>
       </c>
       <c r="AE83" s="2" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="AF83" s="2" t="s">
         <v>19</v>
@@ -14187,7 +14208,7 @@
         <v>21</v>
       </c>
       <c r="AE86" s="2" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="AF86" s="2" t="s">
         <v>19</v>
@@ -14327,8 +14348,8 @@
       <c r="AD87" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AE87" s="14" t="s">
-        <v>48</v>
+      <c r="AE87" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="AF87" s="14" t="s">
         <v>17</v>

</xml_diff>